<commit_message>
added 2 point tasks support
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -536,34 +536,34 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -572,7 +572,7 @@
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -581,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
@@ -617,10 +617,10 @@
         <v>0</v>
       </c>
       <c r="AD2" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AE2" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3">
@@ -635,10 +635,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -662,7 +662,7 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -716,10 +716,10 @@
         <v>0</v>
       </c>
       <c r="AD3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AE3" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
better answer form saving
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,25 +536,25 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
         <v>1</v>
@@ -617,10 +617,10 @@
         <v>0</v>
       </c>
       <c r="AD2" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AE2" t="n">
-        <v>56</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -719,6 +719,303 @@
         <v>0</v>
       </c>
       <c r="AE3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Егор</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Барсуков</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Сергей</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Цыкура</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Фёдор</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Самохин</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
parsing method selection + proto of editable variant
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE6"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,13 +557,13 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -572,7 +572,7 @@
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -581,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
@@ -617,21 +617,21 @@
         <v>0</v>
       </c>
       <c r="AD2" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AE2" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Фёдор</t>
+          <t>Сергей</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Самохин</t>
+          <t>Цыкура</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -725,28 +725,28 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Егор</t>
+          <t>Фёдор</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Барсуков</t>
+          <t>Самохин</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -815,207 +815,9 @@
         <v>0</v>
       </c>
       <c r="AD4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AE4" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Сергей</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Цыкура</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0</v>
-      </c>
-      <c r="V5" t="n">
-        <v>0</v>
-      </c>
-      <c r="W5" t="n">
-        <v>0</v>
-      </c>
-      <c r="X5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>4</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Фёдор</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Самохин</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0</v>
-      </c>
-      <c r="V6" t="n">
-        <v>0</v>
-      </c>
-      <c r="W6" t="n">
-        <v>0</v>
-      </c>
-      <c r="X6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE6" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>